<commit_message>
Small edits to hypotheses file
From chat in early July between Lizzie and Dan
</commit_message>
<xml_diff>
--- a/docs/notes/hypotheses_predictions.xlsx
+++ b/docs/notes/hypotheses_predictions.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27127"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="20520" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="strategies" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="59">
   <si>
     <t>Overall phenology</t>
   </si>
@@ -139,9 +139,6 @@
     <t>Early or late</t>
   </si>
   <si>
-    <t>Higher lead N (why?)</t>
-  </si>
-  <si>
     <t>Highlight which traits in tolerant ARE NOT THE SAME as opportunistic; and which traits in avoider ARE NOT THE SAME as conservative.</t>
   </si>
   <si>
@@ -176,6 +173,30 @@
   </si>
   <si>
     <t xml:space="preserve">File started by Lizzie, based in part off Dan's excellent 'Hypothesis box.' </t>
+  </si>
+  <si>
+    <t>Dan says: Tolerant-avoider is about other functional traits; opprotunistic-conservative is about phenological traits</t>
+  </si>
+  <si>
+    <t>Notes:</t>
+  </si>
+  <si>
+    <t>Height: unimportant</t>
+  </si>
+  <si>
+    <t>Height unimportant</t>
+  </si>
+  <si>
+    <t>Lower leaf N (more structure)</t>
+  </si>
+  <si>
+    <t>No leaf N prediction</t>
+  </si>
+  <si>
+    <t>Updated by Dan some days later</t>
+  </si>
+  <si>
+    <t>Then a couple edits by Lizzie and Dan together in early July</t>
   </si>
 </sst>
 </file>
@@ -690,10 +711,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -830,10 +851,10 @@
         <v>12</v>
       </c>
       <c r="D11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F11" t="s">
         <v>15</v>
@@ -850,10 +871,10 @@
         <v>22</v>
       </c>
       <c r="D12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F12" t="s">
         <v>16</v>
@@ -936,10 +957,10 @@
         <v>27</v>
       </c>
       <c r="F16" t="s">
-        <v>26</v>
+        <v>55</v>
       </c>
       <c r="G16" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -956,40 +977,50 @@
         <v>30</v>
       </c>
       <c r="F17" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="G17" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" t="s">
-        <v>40</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1005,22 +1036,32 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>